<commit_message>
Test: Added unit tests for most ensembleFxns
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="108">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -316,9 +316,6 @@
     <t>m5 m14</t>
   </si>
   <si>
-    <t>putative homotetramer (metacyc). From pdb, might actually be a monomer. Tryptophan is substate inhibitor</t>
-  </si>
-  <si>
     <t>UniUniPromiscuous</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>r2 r5</t>
   </si>
   <si>
-    <t>homodimer (metacyc), inhib by serotonin</t>
-  </si>
-  <si>
     <t>OrdPromiscCompInhibIndep</t>
   </si>
   <si>
@@ -346,9 +340,6 @@
     <t>r3 r6</t>
   </si>
   <si>
-    <t>Serotonin N-acetyltransferase is a monomeric enzyme (metacyc)</t>
-  </si>
-  <si>
     <t>orderedBiBi</t>
   </si>
   <si>
@@ -358,16 +349,7 @@
     <t>m9 m13</t>
   </si>
   <si>
-    <t>ASMT has a C-terminal domain similar to other SAM-dependent O-methyltransferases, and an N-terminal domain which intertwines with another monomer to form the physiologically active dimer  (metacyc); inhib by melatonin</t>
-  </si>
-  <si>
-    <t>Serotonin N-acetyltransferase is a monomeric enzyme (metacyc); inhib by melatonin</t>
-  </si>
-  <si>
     <t>massAction</t>
-  </si>
-  <si>
-    <t>Modeled as mass action</t>
   </si>
   <si>
     <t>diffusion</t>
@@ -509,7 +491,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="L2:O21 B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -642,7 +624,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="L2:O21 A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,7 +770,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1011,7 +993,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1331,17 +1313,17 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5627530364373"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8825910931174"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6720647773279"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
@@ -1406,34 +1388,28 @@
       <c r="K2" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="L2" s="0" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1441,16 +1417,16 @@
         <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>27</v>
@@ -1460,9 +1436,6 @@
       </c>
       <c r="K4" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,22 +1443,19 @@
         <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="L5" s="0" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,25 +1463,22 @@
         <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>2</v>
-      </c>
-      <c r="L6" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,16 +1486,16 @@
         <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>27</v>
@@ -1538,9 +1505,6 @@
       </c>
       <c r="K7" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,7 +1512,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1562,16 +1526,13 @@
         <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K9" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,16 +1540,13 @@
         <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K10" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,16 +1554,13 @@
         <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K11" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,16 +1568,13 @@
         <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K12" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,16 +1582,13 @@
         <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L13" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,16 +1596,13 @@
         <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>1</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1678,7 +1624,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2615,7 +2561,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="L2:O21 D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3062,7 +3008,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="L2:O21 B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3288,7 +3234,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="L2:O21 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3385,7 +3331,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="L2:O21 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3517,7 +3463,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="L2:O21 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3649,7 +3595,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3830,7 +3776,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="L2:O21 H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Tests: updated tests after col names change + numConditions change
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="106">
   <si>
     <t>General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -245,12 +245,6 @@
   </si>
   <si>
     <t>vref_std</t>
-  </si>
-  <si>
-    <t>vexp1_mean</t>
-  </si>
-  <si>
-    <t>vexp1_std</t>
   </si>
   <si>
     <t>enzyme/rxn</t>
@@ -490,8 +484,8 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="1" sqref="L2:O21 B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,18 +615,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="L2:O21 A8"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>68</v>
       </c>
@@ -642,14 +636,8 @@
       <c r="C1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -659,14 +647,8 @@
       <c r="C2" s="0" t="n">
         <v>1.10350536706976</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>-22.0149320730417</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>1.10350536706976</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -676,14 +658,8 @@
       <c r="C3" s="0" t="n">
         <v>2.12397436954052E-007</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>0.285369137837419</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -693,14 +669,8 @@
       <c r="C4" s="0" t="n">
         <v>3.18755368558865E-009</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0.0578197638950879</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -710,14 +680,8 @@
       <c r="C5" s="0" t="n">
         <v>3.33787220043099E-011</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>-0.00439408376660814</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -727,14 +691,8 @@
       <c r="C6" s="0" t="n">
         <v>2.00430304742416E-005</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>6.84865633256387</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -742,12 +700,6 @@
         <v>-0.00242684925806694</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>-0.00242684925806694</v>
-      </c>
-      <c r="E7" s="0" t="n">
         <v>6.60284204552005E-011</v>
       </c>
     </row>
@@ -770,7 +722,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -780,16 +732,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,7 +945,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1006,13 +958,13 @@
         <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,57 +1265,57 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:O21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.8866396761134"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1371,13 +1323,13 @@
         <v>39</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>24</v>
@@ -1394,16 +1346,16 @@
         <v>40</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -1417,16 +1369,16 @@
         <v>41</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>27</v>
@@ -1443,13 +1395,13 @@
         <v>42</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>0</v>
@@ -1463,16 +1415,16 @@
         <v>43</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="J6" s="0" t="n">
         <v>0</v>
@@ -1486,16 +1438,16 @@
         <v>44</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>27</v>
@@ -1512,7 +1464,7 @@
         <v>45</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -1526,7 +1478,7 @@
         <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -1540,7 +1492,7 @@
         <v>47</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -1554,7 +1506,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -1568,7 +1520,7 @@
         <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -1582,7 +1534,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>0</v>
@@ -1596,7 +1548,7 @@
         <v>51</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>0</v>
@@ -1624,7 +1576,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2561,7 +2513,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="1" sqref="L2:O21 D17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3008,7 +2960,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="L2:O21 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3234,7 +3186,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="L2:O21 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3331,7 +3283,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="L2:O21 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3463,7 +3415,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="L2:O21 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3595,7 +3547,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="L2:O21 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3776,7 +3728,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="L2:O21 H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix: fixed fixedExchange + updated respective tests
Now the flux is set explicitly and not hidden in the
enzyme concentrations
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -484,7 +484,7 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1265,17 +1265,17 @@
   </sheetPr>
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="33.1012145748988"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>

</xml_diff>

<commit_message>
Tests: updating tests after TMFA change
Some tests on ensembleFxns are still not working, but most are
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -494,8 +494,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O19" activeCellId="0" sqref="O19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -636,13 +636,16 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,7 +667,8 @@
         <v>-22.0149320730417</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>1.10350536706976</v>
+        <f aca="false">ABS(0.15*B2)</f>
+        <v>3.30223981095625</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,7 +679,8 @@
         <v>0.285369137837419</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>2.12397436954052E-007</v>
+        <f aca="false">ABS(0.15*B3)</f>
+        <v>0.0428053706756129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,7 +691,8 @@
         <v>0.0578197638950879</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>3.18755368558865E-009</v>
+        <f aca="false">ABS(0.15*B4)</f>
+        <v>0.00867296458426318</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,7 +703,8 @@
         <v>-0.00439408376660814</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>3.33787220043099E-011</v>
+        <f aca="false">ABS(0.15*B5)</f>
+        <v>0.000659112564991221</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -708,7 +715,8 @@
         <v>6.84865633256387</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>2.00430304742416E-005</v>
+        <f aca="false">ABS(0.15*B6)</f>
+        <v>1.02729844988458</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -719,7 +727,8 @@
         <v>-0.00242684925806694</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>6.60284204552005E-011</v>
+        <f aca="false">ABS(0.15*B7)</f>
+        <v>0.000364027388710041</v>
       </c>
     </row>
   </sheetData>
@@ -1291,7 +1300,7 @@
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="43.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="42.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.1"/>

</xml_diff>